<commit_message>
Plate for wormgear motor
</commit_message>
<xml_diff>
--- a/NOTES/Budsjett.xlsx
+++ b/NOTES/Budsjett.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UIA\Bachelor\BachelorProsjekt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UIA\Bachelor\BachelorProsjekt\NOTES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E65E91-31CA-46A2-9227-9E7E3BDB8B75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB4BC05D-8DEC-4AF4-A60C-715980A2A746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7ECF43A6-1848-4FDA-8461-36822067C1B7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
   <si>
     <t>Part number</t>
   </si>
@@ -132,6 +132,15 @@
   </si>
   <si>
     <t>Biltema</t>
+  </si>
+  <si>
+    <t>175-5215</t>
+  </si>
+  <si>
+    <t>Total amazon + frakt</t>
+  </si>
+  <si>
+    <t>Sum total kostnad</t>
   </si>
 </sst>
 </file>
@@ -498,8 +507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77625910-4474-448E-B890-7D3021245776}">
   <dimension ref="A2:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -659,25 +668,28 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
       <c r="C12" t="s">
         <v>27</v>
       </c>
       <c r="D12">
-        <v>100</v>
+        <v>77.680000000000007</v>
       </c>
       <c r="E12">
         <v>2</v>
       </c>
       <c r="F12">
         <f>D12*E12</f>
-        <v>200</v>
+        <v>155.36000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="F13">
         <f>SUM(F9:F12)</f>
-        <v>750</v>
+        <v>705.36</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -743,9 +755,6 @@
         <f>D22*E22</f>
         <v>610</v>
       </c>
-      <c r="G22">
-        <v>1</v>
-      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
@@ -767,6 +776,9 @@
       <c r="F24">
         <v>1830</v>
       </c>
+      <c r="G24" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
@@ -830,7 +842,10 @@
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F31">
         <f>F6+F13+F24</f>
-        <v>3720</v>
+        <v>3675.36</v>
+      </c>
+      <c r="G31" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Drawing for bracket bottom and spacer
</commit_message>
<xml_diff>
--- a/NOTES/Budsjett.xlsx
+++ b/NOTES/Budsjett.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UIA\Bachelor\BachelorProsjekt\NOTES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB4BC05D-8DEC-4AF4-A60C-715980A2A746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{913F8A5D-E021-4575-8AD9-95B85A33BB9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7ECF43A6-1848-4FDA-8461-36822067C1B7}"/>
   </bookViews>
@@ -507,8 +507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77625910-4474-448E-B890-7D3021245776}">
   <dimension ref="A2:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -556,11 +556,11 @@
         <v>260</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F3">
         <f>D3*E3</f>
-        <v>520</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -594,17 +594,17 @@
         <v>115</v>
       </c>
       <c r="E5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
-        <v>230</v>
+        <v>460</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F6">
         <f>SUM(F3:F5)</f>
-        <v>1140</v>
+        <v>1890</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -842,7 +842,7 @@
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F31">
         <f>F6+F13+F24</f>
-        <v>3675.36</v>
+        <v>4425.3600000000006</v>
       </c>
       <c r="G31" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
Lagd arbeidstegning av bracketbottom, spacer og monterringsplate
</commit_message>
<xml_diff>
--- a/NOTES/Budsjett.xlsx
+++ b/NOTES/Budsjett.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UIA\Bachelor\BachelorProsjekt\NOTES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{913F8A5D-E021-4575-8AD9-95B85A33BB9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E509B698-B768-42FA-BE8B-2D579D5317C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7ECF43A6-1848-4FDA-8461-36822067C1B7}"/>
   </bookViews>
@@ -508,7 +508,7 @@
   <dimension ref="A2:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Små endringer til monteringsplater osv
</commit_message>
<xml_diff>
--- a/NOTES/Budsjett.xlsx
+++ b/NOTES/Budsjett.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UIA\Bachelor\BachelorProsjekt\NOTES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dngmo\Documents\BachelorProsjekt\NOTES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCDFD997-4169-4E66-8E41-DD1756B01269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92BE7769-AC80-4C95-A4BE-550670A937C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{7ECF43A6-1848-4FDA-8461-36822067C1B7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{7ECF43A6-1848-4FDA-8461-36822067C1B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Budsjett" sheetId="1" r:id="rId1"/>
@@ -249,7 +249,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -551,15 +551,15 @@
       <selection activeCell="K9" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="43" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -582,7 +582,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -603,7 +603,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" t="s">
         <v>7</v>
@@ -622,7 +622,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" t="s">
         <v>10</v>
@@ -641,13 +641,13 @@
         <v>460</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F6">
         <f>SUM(F3:F5)</f>
         <v>1890</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -668,7 +668,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="3">
         <v>51100</v>
@@ -687,7 +687,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" t="s">
         <v>22</v>
@@ -709,7 +709,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" t="s">
         <v>32</v>
@@ -728,14 +728,14 @@
         <v>155.36000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="F13">
         <f>SUM(F9:F12)</f>
         <v>705.36</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" t="s">
         <v>35</v>
@@ -757,7 +757,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" t="s">
         <v>38</v>
@@ -779,28 +779,28 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="F16">
         <f>D16*E16</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>14</v>
       </c>
@@ -818,7 +818,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="C24" t="s">
         <v>24</v>
@@ -834,7 +834,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="C25" t="s">
         <v>25</v>
@@ -850,7 +850,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="C26" t="s">
         <v>26</v>
@@ -866,7 +866,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F27">
         <v>1830</v>
       </c>
@@ -874,7 +874,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>15</v>
       </c>
@@ -895,7 +895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" t="s">
         <v>28</v>
@@ -914,7 +914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" t="s">
         <v>30</v>
@@ -933,7 +933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F34">
         <f>F6+F13+F27</f>
         <v>4425.3600000000006</v>
@@ -953,18 +953,18 @@
   <dimension ref="A2:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="43" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -987,7 +987,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -1008,7 +1008,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" t="s">
         <v>7</v>
@@ -1027,7 +1027,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" t="s">
         <v>10</v>
@@ -1046,18 +1046,18 @@
         <v>460</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F6">
         <f>SUM(F3:F5)</f>
         <v>1890</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>135.36000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="4" t="s">
         <v>38</v>
@@ -1097,7 +1097,7 @@
         <v>321.12</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" t="s">
         <v>22</v>
@@ -1119,7 +1119,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" t="s">
         <v>44</v>
@@ -1138,7 +1138,7 @@
         <v>190.96</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="4" t="s">
         <v>35</v>
@@ -1157,34 +1157,34 @@
         <v>93.5</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="F14">
         <f>SUM(F9:F13)</f>
         <v>823.56000000000006</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>42</v>
       </c>
@@ -1205,7 +1205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="C25" t="s">
         <v>24</v>
@@ -1221,7 +1221,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="C26" t="s">
         <v>25</v>
@@ -1237,7 +1237,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="C27" t="s">
         <v>26</v>
@@ -1253,7 +1253,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F28">
         <v>1830</v>
       </c>
@@ -1261,7 +1261,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>15</v>
       </c>
@@ -1282,7 +1282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" t="s">
         <v>28</v>
@@ -1301,7 +1301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" t="s">
         <v>30</v>
@@ -1320,7 +1320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F35">
         <f>F6+F14+F28</f>
         <v>4543.5599999999995</v>

</xml_diff>

<commit_message>
Noen små oppdateringer på dekselkabelgate
</commit_message>
<xml_diff>
--- a/NOTES/Budsjett.xlsx
+++ b/NOTES/Budsjett.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dngmo\Documents\BachelorProsjekt\NOTES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UIA\Bachelor\BachelorProsjekt\NOTES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92BE7769-AC80-4C95-A4BE-550670A937C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43E2DD59-8285-4042-8007-2CFFF20A605C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{7ECF43A6-1848-4FDA-8461-36822067C1B7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{7ECF43A6-1848-4FDA-8461-36822067C1B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Budsjett" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="47">
   <si>
     <t>Part number</t>
   </si>
@@ -249,7 +249,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -551,15 +551,15 @@
       <selection activeCell="K9" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="43" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -582,7 +582,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -603,7 +603,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" t="s">
         <v>7</v>
@@ -622,7 +622,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" t="s">
         <v>10</v>
@@ -641,13 +641,13 @@
         <v>460</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F6">
         <f>SUM(F3:F5)</f>
         <v>1890</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -668,7 +668,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="3">
         <v>51100</v>
@@ -687,7 +687,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" t="s">
         <v>22</v>
@@ -709,7 +709,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" t="s">
         <v>32</v>
@@ -728,14 +728,14 @@
         <v>155.36000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="F13">
         <f>SUM(F9:F12)</f>
         <v>705.36</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" t="s">
         <v>35</v>
@@ -757,7 +757,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" t="s">
         <v>38</v>
@@ -779,28 +779,28 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="F16">
         <f>D16*E16</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>14</v>
       </c>
@@ -818,7 +818,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="C24" t="s">
         <v>24</v>
@@ -834,7 +834,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="C25" t="s">
         <v>25</v>
@@ -850,7 +850,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="C26" t="s">
         <v>26</v>
@@ -866,7 +866,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F27">
         <v>1830</v>
       </c>
@@ -874,7 +874,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>15</v>
       </c>
@@ -895,7 +895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" t="s">
         <v>28</v>
@@ -914,7 +914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" t="s">
         <v>30</v>
@@ -933,7 +933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F34">
         <f>F6+F13+F27</f>
         <v>4425.3600000000006</v>
@@ -953,18 +953,18 @@
   <dimension ref="A2:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.44140625" customWidth="1"/>
     <col min="7" max="7" width="43" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -987,7 +987,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -1008,7 +1008,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" t="s">
         <v>7</v>
@@ -1027,7 +1027,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" t="s">
         <v>10</v>
@@ -1046,18 +1046,18 @@
         <v>460</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F6">
         <f>SUM(F3:F5)</f>
         <v>1890</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>135.36000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="4" t="s">
         <v>38</v>
@@ -1097,7 +1097,7 @@
         <v>321.12</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" t="s">
         <v>22</v>
@@ -1115,11 +1115,8 @@
         <f>D11*E11</f>
         <v>82.62</v>
       </c>
-      <c r="G11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" t="s">
         <v>44</v>
@@ -1138,7 +1135,7 @@
         <v>190.96</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="4" t="s">
         <v>35</v>
@@ -1157,34 +1154,34 @@
         <v>93.5</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="F14">
         <f>SUM(F9:F13)</f>
         <v>823.56000000000006</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>42</v>
       </c>
@@ -1205,7 +1202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="C25" t="s">
         <v>24</v>
@@ -1221,7 +1218,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="C26" t="s">
         <v>25</v>
@@ -1237,7 +1234,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="C27" t="s">
         <v>26</v>
@@ -1253,7 +1250,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F28">
         <v>1830</v>
       </c>
@@ -1261,7 +1258,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>15</v>
       </c>
@@ -1282,7 +1279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" t="s">
         <v>28</v>
@@ -1301,7 +1298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" t="s">
         <v>30</v>
@@ -1320,7 +1317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F35">
         <f>F6+F14+F28</f>
         <v>4543.5599999999995</v>

</xml_diff>